<commit_message>
added day 2 sql demos
</commit_message>
<xml_diff>
--- a/Training_Plan_SQL_PLSQL_Java.xlsx
+++ b/Training_Plan_SQL_PLSQL_Java.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chainsys-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF08264E-20B0-4736-AF17-67CE4D95DC02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D62D730-9F8B-4389-B5FB-0CAB62936662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D62FE30-D1C8-4249-B075-89814755D9EA}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D62FE30-D1C8-4249-B075-89814755D9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL" sheetId="1" r:id="rId1"/>
@@ -992,85 +992,85 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1387,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBC4422-F2CD-4B8D-9A44-F3781D4A65DD}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1408,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="50" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1419,7 +1419,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +1428,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1464,8 +1464,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="60" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1473,7 +1473,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="12" t="s">
         <v>45</v>
       </c>
@@ -1496,7 +1496,7 @@
       <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="2" t="s">
         <v>52</v>
       </c>
@@ -1543,8 +1543,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="60" t="s">
+      <c r="A17" s="51"/>
+      <c r="B17" s="40" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="12" t="s">
         <v>45</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="53" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1586,7 +1586,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1595,97 +1595,97 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="40"/>
+      <c r="C24" s="49"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="40"/>
+      <c r="C25" s="49"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="40"/>
+      <c r="C27" s="49"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="40"/>
+      <c r="C28" s="49"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="40"/>
+      <c r="C29" s="49"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="40"/>
+      <c r="C30" s="49"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="40"/>
+      <c r="C32" s="49"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="51"/>
       <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="40"/>
+      <c r="C33" s="49"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="40"/>
+      <c r="C34" s="49"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="51"/>
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="51"/>
       <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="43"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="12" t="s">
         <v>45</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="C38" s="19"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="53" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="2" t="s">
         <v>31</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="2" t="s">
         <v>32</v>
       </c>
@@ -1746,7 +1746,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="2" t="s">
         <v>33</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="2" t="s">
         <v>34</v>
       </c>
@@ -1764,23 +1764,23 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="40"/>
+      <c r="C45" s="49"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="2" t="s">
         <v>36</v>
       </c>
@@ -1789,7 +1789,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
+      <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="43"/>
+      <c r="A48" s="52"/>
       <c r="B48" s="12" t="s">
         <v>45</v>
       </c>
@@ -1812,99 +1812,99 @@
       <c r="C49" s="19"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="61" t="s">
+      <c r="A50" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="43" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="63"/>
-      <c r="B51" s="60" t="s">
+      <c r="A51" s="47"/>
+      <c r="B51" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="67" t="s">
+      <c r="C51" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="63"/>
-      <c r="B52" s="60" t="s">
+      <c r="A52" s="47"/>
+      <c r="B52" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="67" t="s">
+      <c r="C52" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="63"/>
-      <c r="B53" s="60" t="s">
+      <c r="A53" s="47"/>
+      <c r="B53" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="67" t="s">
+      <c r="C53" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="63"/>
-      <c r="B54" s="60" t="s">
+      <c r="A54" s="47"/>
+      <c r="B54" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="67" t="s">
+      <c r="C54" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="63"/>
-      <c r="B55" s="60" t="s">
+      <c r="A55" s="47"/>
+      <c r="B55" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="67" t="s">
+      <c r="C55" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="63"/>
-      <c r="B56" s="60" t="s">
+      <c r="A56" s="47"/>
+      <c r="B56" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="67" t="s">
+      <c r="C56" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="63"/>
-      <c r="B57" s="60" t="s">
+      <c r="A57" s="47"/>
+      <c r="B57" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="67" t="s">
+      <c r="C57" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="64"/>
-      <c r="B58" s="65" t="s">
+      <c r="A58" s="48"/>
+      <c r="B58" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C58" s="45" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A21:A37"/>
+    <mergeCell ref="A39:A48"/>
     <mergeCell ref="A50:A58"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A21:A37"/>
-    <mergeCell ref="A39:A48"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1915,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB60A59-42D1-489B-A98B-8CA6626826F3}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="54" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -2028,30 +2028,30 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="49"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="49"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="2" t="s">
         <v>64</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="2" t="s">
         <v>65</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="2" t="s">
         <v>66</v>
       </c>
@@ -2078,53 +2078,53 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="49"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="49"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="49"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="55"/>
       <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="12" t="s">
         <v>45</v>
       </c>
@@ -2147,7 +2147,7 @@
       <c r="C26" s="22"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="54" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -2158,7 +2158,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="2" t="s">
         <v>74</v>
       </c>
@@ -2167,7 +2167,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="2" t="s">
         <v>75</v>
       </c>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="2" t="s">
         <v>80</v>
       </c>
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="2" t="s">
         <v>76</v>
       </c>
@@ -2194,7 +2194,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="2" t="s">
         <v>77</v>
       </c>
@@ -2203,7 +2203,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2212,7 +2212,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="2" t="s">
         <v>79</v>
       </c>
@@ -2221,7 +2221,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="2" t="s">
         <v>49</v>
       </c>
@@ -2230,7 +2230,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="12" t="s">
         <v>45</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="C37" s="22"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="54" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -2255,7 +2255,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="2" t="s">
         <v>81</v>
       </c>
@@ -2264,7 +2264,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="6" t="s">
         <v>82</v>
       </c>
@@ -2273,7 +2273,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="6" t="s">
         <v>87</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
+      <c r="A42" s="55"/>
       <c r="B42" s="7" t="s">
         <v>86</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="46"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="7" t="s">
         <v>83</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
+      <c r="A44" s="55"/>
       <c r="B44" s="7" t="s">
         <v>84</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="2" t="s">
         <v>49</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="47"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="12" t="s">
         <v>45</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="C47" s="22"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="54" t="s">
         <v>29</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -2343,39 +2343,39 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="46"/>
+      <c r="A49" s="55"/>
       <c r="B49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
+      <c r="A50" s="55"/>
       <c r="B50" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="40"/>
+      <c r="C50" s="49"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="40"/>
+      <c r="C52" s="49"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="46"/>
+      <c r="A53" s="55"/>
       <c r="B53" s="7" t="s">
         <v>92</v>
       </c>
@@ -2384,7 +2384,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
+      <c r="A54" s="55"/>
       <c r="B54" s="7" t="s">
         <v>94</v>
       </c>
@@ -2393,23 +2393,23 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="46"/>
+      <c r="A55" s="55"/>
       <c r="B55" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="49" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
+      <c r="A56" s="55"/>
       <c r="B56" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="40"/>
+      <c r="C56" s="49"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
+      <c r="A57" s="55"/>
       <c r="B57" s="7" t="s">
         <v>97</v>
       </c>
@@ -2418,7 +2418,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="2" t="s">
         <v>49</v>
       </c>
@@ -2427,7 +2427,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="47"/>
+      <c r="A59" s="56"/>
       <c r="B59" s="12" t="s">
         <v>45</v>
       </c>
@@ -2440,6 +2440,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A48:A59"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C55:C56"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A27:A36"/>
     <mergeCell ref="A38:A46"/>
@@ -2447,10 +2451,6 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A48:A59"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C55:C56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2460,8 +2460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0C643F-02D9-4618-88D0-100C6382785A}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="53" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2492,95 +2492,95 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="49" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="40"/>
+      <c r="C5" s="49"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="49"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="49" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="49"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="49"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="49"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="49"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="49"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="49"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="4" t="s">
         <v>49</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="36" t="s">
         <v>45</v>
       </c>
@@ -2603,7 +2603,7 @@
       <c r="C17" s="38"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2614,65 +2614,65 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="57" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="58"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="58"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="58"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="58"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="58"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="58"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="50"/>
+      <c r="C26" s="59"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
@@ -2681,7 +2681,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
+      <c r="A28" s="66"/>
       <c r="B28" s="4" t="s">
         <v>45</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="C29" s="33"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="67" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="35" t="s">
@@ -2706,146 +2706,146 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="58" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="49"/>
+      <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="49"/>
+      <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="50"/>
+      <c r="C34" s="59"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="60" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="52"/>
+      <c r="C36" s="61"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="52"/>
+      <c r="C37" s="61"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="52"/>
+      <c r="C38" s="61"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="52"/>
+      <c r="C39" s="61"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C40" s="52"/>
+      <c r="C40" s="61"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C41" s="53"/>
+      <c r="C41" s="62"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="55"/>
+      <c r="C43" s="64"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
+      <c r="A44" s="68"/>
       <c r="B44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="55"/>
+      <c r="C44" s="64"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
+      <c r="A45" s="68"/>
       <c r="B45" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="55"/>
+      <c r="C45" s="64"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
+      <c r="A46" s="68"/>
       <c r="B46" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="55"/>
+      <c r="C46" s="64"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
+      <c r="A47" s="68"/>
       <c r="B47" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C47" s="55"/>
+      <c r="C47" s="64"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
+      <c r="A48" s="68"/>
       <c r="B48" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="55"/>
+      <c r="C48" s="64"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="59"/>
+      <c r="A49" s="68"/>
       <c r="B49" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C49" s="56"/>
+      <c r="C49" s="65"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="59"/>
+      <c r="A50" s="68"/>
       <c r="B50" s="4" t="s">
         <v>49</v>
       </c>
@@ -2854,7 +2854,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="59"/>
+      <c r="A51" s="68"/>
       <c r="B51" s="36" t="s">
         <v>45</v>
       </c>
@@ -2868,7 +2868,7 @@
       <c r="C52" s="19"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="54" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -2879,67 +2879,67 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
+      <c r="A54" s="55"/>
       <c r="B54" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="49" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="46"/>
+      <c r="A55" s="55"/>
       <c r="B55" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="40"/>
+      <c r="C55" s="49"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
+      <c r="A56" s="55"/>
       <c r="B56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="40"/>
+      <c r="C56" s="49"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
+      <c r="A57" s="55"/>
       <c r="B57" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C57" s="40"/>
+      <c r="C57" s="49"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C58" s="37"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="49" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="46"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="40"/>
+      <c r="C60" s="49"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="46"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="40"/>
+      <c r="C61" s="49"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="46"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="4" t="s">
         <v>49</v>
       </c>
@@ -2948,7 +2948,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="47"/>
+      <c r="A63" s="56"/>
       <c r="B63" s="36" t="s">
         <v>45</v>
       </c>
@@ -2962,7 +2962,7 @@
       <c r="C64" s="19"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="s">
+      <c r="A65" s="53" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -2973,51 +2973,51 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="60" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
+      <c r="A67" s="51"/>
       <c r="B67" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C67" s="52"/>
+      <c r="C67" s="61"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="42"/>
+      <c r="A68" s="51"/>
       <c r="B68" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="52"/>
+      <c r="C68" s="61"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="42"/>
+      <c r="A69" s="51"/>
       <c r="B69" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C69" s="52"/>
+      <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
+      <c r="A70" s="51"/>
       <c r="B70" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C70" s="52"/>
+      <c r="C70" s="61"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="42"/>
+      <c r="A71" s="51"/>
       <c r="B71" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C71" s="53"/>
+      <c r="C71" s="62"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="42"/>
+      <c r="A72" s="51"/>
       <c r="B72" s="4" t="s">
         <v>49</v>
       </c>
@@ -3026,7 +3026,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="43"/>
+      <c r="A73" s="52"/>
       <c r="B73" s="36" t="s">
         <v>45</v>
       </c>

</xml_diff>